<commit_message>
Mean Frequency and Standard Deviation for frequency results
</commit_message>
<xml_diff>
--- a/Frequency/Results/dec_to_march_2013.xlsx
+++ b/Frequency/Results/dec_to_march_2013.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eren\Desktop\teias_freq\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eren\Desktop\github\Researchh\Frequency\Results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -2074,18 +2074,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:D98"/>
+  <dimension ref="A2:E98"/>
   <sheetViews>
-    <sheetView topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="A59" sqref="A2:D98"/>
+    <sheetView topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
+    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -2098,8 +2099,11 @@
       <c r="D2">
         <v>2.2206116462525162E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" s="1">
+        <v>41244</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2112,8 +2116,11 @@
       <c r="D3">
         <v>2.1267876792832738E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3" s="1">
+        <v>41245</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2126,8 +2133,11 @@
       <c r="D4">
         <v>2.6650145211543096E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4" s="1">
+        <v>41246</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2140,8 +2150,11 @@
       <c r="D5">
         <v>2.5109569093252865E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5" s="1">
+        <v>41247</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -2154,8 +2167,11 @@
       <c r="D6">
         <v>2.2803744211141685E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6" s="1">
+        <v>41248</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -2168,8 +2184,11 @@
       <c r="D7">
         <v>2.4265739725872329E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7" s="1">
+        <v>41249</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -2182,8 +2201,11 @@
       <c r="D8">
         <v>2.3724753597585423E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" s="1">
+        <v>41250</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -2196,8 +2218,11 @@
       <c r="D9">
         <v>2.2503513600442764E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" s="1">
+        <v>41251</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -2210,8 +2235,11 @@
       <c r="D10">
         <v>2.2471825649025653E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" s="1">
+        <v>41252</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -2224,8 +2252,11 @@
       <c r="D11">
         <v>2.3364659434324381E-2</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" s="1">
+        <v>41253</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -2238,8 +2269,11 @@
       <c r="D12">
         <v>2.4986985673181153E-2</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12" s="1">
+        <v>41254</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -2252,8 +2286,11 @@
       <c r="D13">
         <v>2.267970857295442E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13" s="1">
+        <v>41255</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -2266,8 +2303,11 @@
       <c r="D14">
         <v>2.3852584162606858E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14" s="1">
+        <v>41256</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -2280,8 +2320,11 @@
       <c r="D15">
         <v>2.361020452938872E-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15" s="1">
+        <v>41257</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -2294,8 +2337,11 @@
       <c r="D16">
         <v>1.9127451845301291E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" s="1">
+        <v>41258</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -2308,8 +2354,11 @@
       <c r="D17">
         <v>2.0023059876855518E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" s="1">
+        <v>41259</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -2322,8 +2371,11 @@
       <c r="D18">
         <v>2.21192008468457E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" s="1">
+        <v>41260</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -2336,8 +2388,11 @@
       <c r="D19">
         <v>2.3191783612813679E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" s="1">
+        <v>41261</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -2350,8 +2405,11 @@
       <c r="D20">
         <v>2.4377926893048005E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" s="1">
+        <v>41262</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -2364,8 +2422,11 @@
       <c r="D21">
         <v>2.401002435551023E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" s="1">
+        <v>41263</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -2378,8 +2439,11 @@
       <c r="D22">
         <v>2.1235648187142964E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" s="1">
+        <v>41264</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -2392,8 +2456,11 @@
       <c r="D23">
         <v>2.0457429573297031E-2</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" s="1">
+        <v>41265</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -2406,8 +2473,11 @@
       <c r="D24">
         <v>1.8967043897892638E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" s="1">
+        <v>41266</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -2420,8 +2490,11 @@
       <c r="D25">
         <v>2.9641804766150519E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" s="1">
+        <v>41267</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -2434,8 +2507,11 @@
       <c r="D26">
         <v>1.7522806758441152E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" s="1">
+        <v>41268</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2448,8 +2524,11 @@
       <c r="D27">
         <v>1.7406760211467687E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" s="1">
+        <v>41269</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2462,8 +2541,11 @@
       <c r="D28">
         <v>2.0935341460065725E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" s="1">
+        <v>41270</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2476,8 +2558,11 @@
       <c r="D29">
         <v>1.9180182146793852E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" s="1">
+        <v>41271</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2490,8 +2575,11 @@
       <c r="D30">
         <v>1.8773702877348211E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30" s="1">
+        <v>41272</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2504,8 +2592,11 @@
       <c r="D31">
         <v>1.7653000889214961E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31" s="1">
+        <v>41273</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2518,8 +2609,11 @@
       <c r="D32">
         <v>1.9972908274176995E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32" s="1">
+        <v>41274</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2532,8 +2626,11 @@
       <c r="D33">
         <v>1.9889899959205082E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33" s="1">
+        <v>41275</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2546,8 +2643,11 @@
       <c r="D34">
         <v>1.9397895400242251E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34" s="1">
+        <v>41276</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -2560,8 +2660,11 @@
       <c r="D35">
         <v>2.0343171466055396E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35" s="1">
+        <v>41277</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2574,8 +2677,11 @@
       <c r="D36">
         <v>1.9960274336378172E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36" s="1">
+        <v>41278</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -2588,8 +2694,11 @@
       <c r="D37">
         <v>1.9931857459583379E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37" s="1">
+        <v>41279</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2602,8 +2711,11 @@
       <c r="D38">
         <v>2.1485088828387341E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38" s="1">
+        <v>41280</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -2616,8 +2728,11 @@
       <c r="D39">
         <v>2.1376938559693373E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39" s="1">
+        <v>41281</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -2630,8 +2745,11 @@
       <c r="D40">
         <v>2.3226467970809492E-2</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40" s="1">
+        <v>41282</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -2644,8 +2762,11 @@
       <c r="D41">
         <v>2.3208480423171779E-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41" s="1">
+        <v>41283</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -2658,8 +2779,11 @@
       <c r="D42">
         <v>2.1351995051442172E-2</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42" s="1">
+        <v>41284</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -2672,8 +2796,11 @@
       <c r="D43">
         <v>2.5211334069279896E-2</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43" s="1">
+        <v>41285</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2686,8 +2813,11 @@
       <c r="D44">
         <v>2.0579054543441416E-2</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44" s="1">
+        <v>41286</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -2700,8 +2830,11 @@
       <c r="D45">
         <v>1.9672169308046487E-2</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45" s="1">
+        <v>41287</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>44</v>
       </c>
@@ -2714,8 +2847,11 @@
       <c r="D46">
         <v>2.2153476652191868E-2</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46" s="1">
+        <v>41288</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>45</v>
       </c>
@@ -2728,8 +2864,11 @@
       <c r="D47">
         <v>2.1919647745864367E-2</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47" s="1">
+        <v>41289</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>46</v>
       </c>
@@ -2742,8 +2881,11 @@
       <c r="D48">
         <v>2.2918250455209961E-2</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48" s="1">
+        <v>41290</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>47</v>
       </c>
@@ -2756,8 +2898,11 @@
       <c r="D49">
         <v>2.4582998450130535E-2</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49" s="1">
+        <v>41291</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>48</v>
       </c>
@@ -2770,8 +2915,11 @@
       <c r="D50">
         <v>2.689962636471983E-2</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50" s="1">
+        <v>41292</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>49</v>
       </c>
@@ -2784,8 +2932,11 @@
       <c r="D51">
         <v>2.5437186346879026E-2</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51" s="1">
+        <v>41293</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>50</v>
       </c>
@@ -2798,8 +2949,11 @@
       <c r="D52">
         <v>2.3867955490518265E-2</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52" s="1">
+        <v>41294</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>51</v>
       </c>
@@ -2812,8 +2966,11 @@
       <c r="D53">
         <v>2.8595577143491851E-2</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53" s="1">
+        <v>41295</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>52</v>
       </c>
@@ -2826,8 +2983,11 @@
       <c r="D54">
         <v>2.5869389467167908E-2</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54" s="1">
+        <v>41296</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>53</v>
       </c>
@@ -2840,8 +3000,11 @@
       <c r="D55">
         <v>2.4859134803736655E-2</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55" s="1">
+        <v>41297</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>54</v>
       </c>
@@ -2854,8 +3017,11 @@
       <c r="D56">
         <v>2.4043269496035958E-2</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56" s="1">
+        <v>41298</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>55</v>
       </c>
@@ -2868,8 +3034,11 @@
       <c r="D57">
         <v>2.4606614467952592E-2</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57" s="1">
+        <v>41299</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>56</v>
       </c>
@@ -2877,7 +3046,7 @@
         <v>1E-3</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>57</v>
       </c>
@@ -2891,7 +3060,7 @@
         <v>2.036669776323816E-2</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>58</v>
       </c>
@@ -2905,7 +3074,7 @@
         <v>2.2482857189934521E-2</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>59</v>
       </c>
@@ -2919,7 +3088,7 @@
         <v>2.3347552351094921E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>60</v>
       </c>
@@ -2933,7 +3102,7 @@
         <v>2.3728881408182904E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>61</v>
       </c>
@@ -2947,7 +3116,7 @@
         <v>2.2798440766945777E-2</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>62</v>
       </c>
@@ -3440,8 +3609,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>